<commit_message>
AOS create new - updated
</commit_message>
<xml_diff>
--- a/AOS Create New User/Default.xlsx
+++ b/AOS Create New User/Default.xlsx
@@ -17,13 +17,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
   <si>
-    <t>usmandemo4</t>
+    <t>usmandemo7</t>
   </si>
   <si>
     <t>New Users</t>
   </si>
   <si>
-    <t>usmandemo5</t>
+    <t>usmandemo8</t>
   </si>
   <si>
     <t>usmandemo6</t>
@@ -503,7 +503,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>

</xml_diff>